<commit_message>
13:37 time 15.03.2024 day
</commit_message>
<xml_diff>
--- a/file_service/person.xlsx
+++ b/file_service/person.xlsx
@@ -398,7 +398,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G1" sqref="G1"/>
@@ -699,6 +699,154 @@
         </is>
       </c>
     </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Ganiyva Nafisaxon Sardor qizi</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>998994884859</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>994884859</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>23 maktab</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>8 yosh</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Isoqov Eldor Fayzullayevich</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>998971300087</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>eldorisoqov</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>971300087</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>45</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>37</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Isoqov Eldor Fayzullayevich</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>998971300087</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>eldorisoqov</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>971300087</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>45</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>998971300087</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>eldorisoqov</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>97 130 00 87</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>45</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>37</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>